<commit_message>
maj squellette plus debut import sprite
</commit_message>
<xml_diff>
--- a/Doc/estimation_felixil.xlsx
+++ b/Doc/estimation_felixil.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="48">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Temps (h)</t>
+  </si>
+  <si>
+    <t>continuer squellete(3h)popup login(2h)tutoriel Sprite(3h)recherche img(3h)</t>
+  </si>
+  <si>
+    <t>séparé img sprite (2h)</t>
   </si>
 </sst>
 </file>
@@ -1610,8 +1616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C3" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="C14" zoomScale="85" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1619,7 +1625,7 @@
     <col min="1" max="1" width="3.44140625" customWidth="1"/>
     <col min="2" max="2" width="64.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41.21875" customWidth="1"/>
+    <col min="6" max="6" width="58.77734375" customWidth="1"/>
     <col min="7" max="8" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1708,8 +1714,12 @@
       <c r="E17" s="18">
         <v>43128</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G17" s="3">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="10">
@@ -1724,8 +1734,12 @@
       <c r="E18" s="18">
         <v>43129</v>
       </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="3"/>
+      <c r="F18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
@@ -1774,7 +1788,7 @@
       <c r="F21" s="20"/>
       <c r="G21" s="11">
         <f>SUM(G16:G20)</f>
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -1938,7 +1952,7 @@
       </c>
       <c r="F36" s="5" t="str">
         <f>IF(G21+G34&lt;90,"Il manque "&amp;90-(G21+G34)&amp;"h",IF(G21+G34&gt;90,"Il y a "&amp;(G21+G34)-90&amp;"h de trop",""))</f>
-        <v>Il manque 82h</v>
+        <v>Il manque 69h</v>
       </c>
     </row>
   </sheetData>

</xml_diff>